<commit_message>
Quests can now take copper coins.
- Added new quests, items, fixes and test updates.
</commit_message>
<xml_diff>
--- a/resources/data-imports/items/QuestItems.xlsx
+++ b/resources/data-imports/items/QuestItems.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="241">
   <si>
     <t>item_suffix_id</t>
   </si>
@@ -708,6 +708,36 @@
   </si>
   <si>
     <t>get-copper-coins</t>
+  </si>
+  <si>
+    <t>Musty old Church Records</t>
+  </si>
+  <si>
+    <t>These old Church records state that alchemy was apart of the Church in one way or another. It seems, if I can make out these musty old pages, that the Church tried to use Holy magic and Alchemy to create special types of candles.</t>
+  </si>
+  <si>
+    <t>Alchemically Enchanted Holy Candle</t>
+  </si>
+  <si>
+    <t>This item will let you ignore the Leveling caps and gain XP faster.</t>
+  </si>
+  <si>
+    <t>Dried up Enchanted Holy Ink</t>
+  </si>
+  <si>
+    <t>This old ink was used to write enchantments on candles back when the Church was still a thing through out Tlessa, fanatical bunch if you ask me. They created these types of enchanted "Holy Inks" that only the elite could get their hands on. The Candle Maker might be able to make use of this.</t>
+  </si>
+  <si>
+    <t>Fanatics Candle of Despair</t>
+  </si>
+  <si>
+    <t>Well, I guess that ink you had found was a bit cursed. But this should still do the trick child. I think ...</t>
+  </si>
+  <si>
+    <t>Corrupted Candle of the Church</t>
+  </si>
+  <si>
+    <t>Well it's become corrupted, the alchemical process failed, but it seems to be emanating a strange glow of power.</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1073,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BF71"/>
+  <dimension ref="A1:BF76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1054,7 +1084,7 @@
     <col min="1" max="1" width="17" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="17" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="37" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="41" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="6" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="370" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="19" bestFit="true" customWidth="true" style="0"/>
@@ -6074,6 +6104,157 @@
         <v>230</v>
       </c>
     </row>
+    <row r="72" spans="1:58">
+      <c r="D72" t="s">
+        <v>231</v>
+      </c>
+      <c r="E72" t="s">
+        <v>59</v>
+      </c>
+      <c r="F72" t="s">
+        <v>232</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="V72">
+        <v>0</v>
+      </c>
+      <c r="W72">
+        <v>0</v>
+      </c>
+      <c r="BD72" t="s">
+        <v>153</v>
+      </c>
+      <c r="BE72">
+        <v>0.05</v>
+      </c>
+      <c r="BF72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:58">
+      <c r="D73" t="s">
+        <v>233</v>
+      </c>
+      <c r="E73" t="s">
+        <v>59</v>
+      </c>
+      <c r="F73" t="s">
+        <v>234</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="V73">
+        <v>0</v>
+      </c>
+      <c r="W73">
+        <v>0</v>
+      </c>
+      <c r="BE73">
+        <v>0.95</v>
+      </c>
+      <c r="BF73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:58">
+      <c r="D74" t="s">
+        <v>235</v>
+      </c>
+      <c r="E74" t="s">
+        <v>59</v>
+      </c>
+      <c r="F74" t="s">
+        <v>236</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="V74">
+        <v>0</v>
+      </c>
+      <c r="W74">
+        <v>0</v>
+      </c>
+      <c r="BD74" t="s">
+        <v>167</v>
+      </c>
+      <c r="BE74">
+        <v>0.15</v>
+      </c>
+      <c r="BF74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:58">
+      <c r="D75" t="s">
+        <v>237</v>
+      </c>
+      <c r="E75" t="s">
+        <v>59</v>
+      </c>
+      <c r="F75" t="s">
+        <v>238</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="V75">
+        <v>0</v>
+      </c>
+      <c r="W75">
+        <v>0</v>
+      </c>
+      <c r="BE75">
+        <v>1.25</v>
+      </c>
+      <c r="BF75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:58">
+      <c r="D76" t="s">
+        <v>239</v>
+      </c>
+      <c r="E76" t="s">
+        <v>59</v>
+      </c>
+      <c r="F76" t="s">
+        <v>240</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="V76">
+        <v>0</v>
+      </c>
+      <c r="W76">
+        <v>0</v>
+      </c>
+      <c r="BE76">
+        <v>1.6</v>
+      </c>
+      <c r="BF76">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>

<commit_message>
Updated quest items and quests.
</commit_message>
<xml_diff>
--- a/resources/data-imports/items/QuestItems.xlsx
+++ b/resources/data-imports/items/QuestItems.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="261">
   <si>
     <t>item_suffix_id</t>
   </si>
@@ -191,6 +191,12 @@
     <t>ignores_caps</t>
   </si>
   <si>
+    <t>can_use_on_other_items</t>
+  </si>
+  <si>
+    <t>holy_level</t>
+  </si>
+  <si>
     <t>Weapon Smiths Book</t>
   </si>
   <si>
@@ -738,6 +744,60 @@
   </si>
   <si>
     <t>Well it's become corrupted, the alchemical process failed, but it seems to be emanating a strange glow of power.</t>
+  </si>
+  <si>
+    <t>Purgatory Smiths House Key</t>
+  </si>
+  <si>
+    <t>Lets you enter the house of the purgatory smith.</t>
+  </si>
+  <si>
+    <t>Smithies Hammer</t>
+  </si>
+  <si>
+    <t>This hammer belonged to the Blacksmith, but what is he doing out of Purgatory?</t>
+  </si>
+  <si>
+    <t>Smithies Iron Chunks</t>
+  </si>
+  <si>
+    <t>Funny that these should be found on surface. First his hammer is in Dungeons and now some of his components are on surface. What is happening?</t>
+  </si>
+  <si>
+    <t>Broken Smithies Anvil</t>
+  </si>
+  <si>
+    <t>How is this in the Wrecked Ship? What is going on? Someone scattered all the smithies tools across the various planes. Was it the Creator?</t>
+  </si>
+  <si>
+    <t>Smithies Dying Ember</t>
+  </si>
+  <si>
+    <t>Satans cage holds a lot of interesting things to say the least, how ever why is the Smithies Dying Ember here? Something smells off child.</t>
+  </si>
+  <si>
+    <t>Candle of the Smithy</t>
+  </si>
+  <si>
+    <t>This unique looking candle has some enchanted engravings on it ... Wait a minute, these are not just any engravings. Apparently, according to these etchings in the wax, "After The Creator escaped Purgatory, he stole the tools of the smithy and scattered them around the various planes So that no one could create the items needed to take down The Creator." Or something to that effect.</t>
+  </si>
+  <si>
+    <t>Vial of Water from the well of the Smith</t>
+  </si>
+  <si>
+    <t>What an interesting and unique item to say the least child. Maybe the candle maker can make use of it?</t>
+  </si>
+  <si>
+    <t>Purgatories Cursed Candle</t>
+  </si>
+  <si>
+    <t>Having the Candle Maker apply the vial of water to this candle of yours has corrupted it further, but it seems to have done the trick. Enemies will have a harder time voiding you now.</t>
+  </si>
+  <si>
+    <t>Bag of Transformation</t>
+  </si>
+  <si>
+    <t>I have heard of this item child, it's used to combine a whole bunch of items into a single item. Maybe this is what is needed, in conjunction with all the other Smithy items you have been finding.</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1133,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BF76"/>
+  <dimension ref="A1:BH85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1084,9 +1144,9 @@
     <col min="1" max="1" width="17" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="17" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="41" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="48" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="6" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="370" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="455" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="19" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="15" bestFit="true" customWidth="true" style="0"/>
@@ -1139,9 +1199,11 @@
     <col min="56" max="56" width="24" bestFit="true" customWidth="true" style="0"/>
     <col min="57" max="57" width="10" bestFit="true" customWidth="true" style="0"/>
     <col min="58" max="58" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="59" max="59" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="60" max="60" width="12" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58">
+    <row r="1" spans="1:60">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1316,22 +1378,28 @@
       <c r="BF1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:58">
+      <c r="BG1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:60">
       <c r="D2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="Z2">
         <v>1</v>
       </c>
       <c r="AD2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AE2">
         <v>0.15</v>
@@ -1388,21 +1456,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:58">
+    <row r="3" spans="1:60">
       <c r="D3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Z3">
         <v>1</v>
       </c>
       <c r="AD3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AE3">
         <v>0.15</v>
@@ -1459,18 +1527,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:58">
+    <row r="4" spans="1:60">
       <c r="D4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="X4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Z4">
         <v>1</v>
@@ -1524,21 +1592,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:58">
+    <row r="5" spans="1:60">
       <c r="D5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="Z5">
         <v>1</v>
       </c>
       <c r="AD5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AE5">
         <v>0.15</v>
@@ -1595,21 +1663,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:58">
+    <row r="6" spans="1:60">
       <c r="D6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Z6">
         <v>1</v>
       </c>
       <c r="AD6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AE6">
         <v>0.15</v>
@@ -1666,21 +1734,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:58">
+    <row r="7" spans="1:60">
       <c r="D7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="Z7">
         <v>1</v>
       </c>
       <c r="AD7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AE7">
         <v>0.15</v>
@@ -1737,21 +1805,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:58">
+    <row r="8" spans="1:60">
       <c r="D8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Z8">
         <v>1</v>
       </c>
       <c r="AD8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="AE8">
         <v>0.15</v>
@@ -1808,18 +1876,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:58">
+    <row r="9" spans="1:60">
       <c r="D9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="X9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z9">
         <v>1</v>
@@ -1873,15 +1941,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:58">
+    <row r="10" spans="1:60">
       <c r="D10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1890,7 +1958,7 @@
         <v>0</v>
       </c>
       <c r="X10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Z10">
         <v>1</v>
@@ -1944,15 +2012,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:58">
+    <row r="11" spans="1:60">
       <c r="D11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1961,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="X11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AF11">
         <v>0</v>
@@ -2012,15 +2080,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:58">
+    <row r="12" spans="1:60">
       <c r="D12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -2029,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="X12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AF12">
         <v>0</v>
@@ -2080,15 +2148,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:58">
+    <row r="13" spans="1:60">
       <c r="D13" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -2148,15 +2216,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:58">
+    <row r="14" spans="1:60">
       <c r="D14" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F14" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -2216,15 +2284,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:58">
+    <row r="15" spans="1:60">
       <c r="D15" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -2236,7 +2304,7 @@
         <v>1</v>
       </c>
       <c r="AD15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="AE15">
         <v>0.5</v>
@@ -2293,15 +2361,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:58">
+    <row r="16" spans="1:60">
       <c r="D16" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -2313,7 +2381,7 @@
         <v>1</v>
       </c>
       <c r="AD16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AE16">
         <v>0.5</v>
@@ -2370,15 +2438,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:58">
+    <row r="17" spans="1:60">
       <c r="D17" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -2390,7 +2458,7 @@
         <v>1</v>
       </c>
       <c r="AD17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AE17">
         <v>0.5</v>
@@ -2447,15 +2515,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:58">
+    <row r="18" spans="1:60">
       <c r="D18" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -2467,7 +2535,7 @@
         <v>1</v>
       </c>
       <c r="AD18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AE18">
         <v>0.5</v>
@@ -2524,15 +2592,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:58">
+    <row r="19" spans="1:60">
       <c r="D19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -2544,7 +2612,7 @@
         <v>1</v>
       </c>
       <c r="AD19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AE19">
         <v>0.5</v>
@@ -2601,15 +2669,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:58">
+    <row r="20" spans="1:60">
       <c r="D20" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -2618,7 +2686,7 @@
         <v>0</v>
       </c>
       <c r="AD20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AE20">
         <v>0.5</v>
@@ -2675,15 +2743,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:58">
+    <row r="21" spans="1:60">
       <c r="D21" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -2743,15 +2811,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:58">
+    <row r="22" spans="1:60">
       <c r="D22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F22" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2760,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="X22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AF22">
         <v>0</v>
@@ -2811,15 +2879,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:58">
+    <row r="23" spans="1:60">
       <c r="D23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -2834,7 +2902,7 @@
         <v>0</v>
       </c>
       <c r="AD23" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AE23">
         <v>0.45</v>
@@ -2891,15 +2959,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:58">
+    <row r="24" spans="1:60">
       <c r="D24" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F24" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -2914,7 +2982,7 @@
         <v>0</v>
       </c>
       <c r="AD24" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AE24">
         <v>0.45</v>
@@ -2971,15 +3039,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:58">
+    <row r="25" spans="1:60">
       <c r="D25" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F25" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -2994,7 +3062,7 @@
         <v>0</v>
       </c>
       <c r="X25" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AF25">
         <v>0</v>
@@ -3045,30 +3113,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:58">
+    <row r="26" spans="1:60">
       <c r="D26" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F26" t="s">
+        <v>125</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26" t="s">
         <v>123</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="V26">
-        <v>0</v>
-      </c>
-      <c r="W26">
-        <v>0</v>
-      </c>
-      <c r="X26" t="s">
-        <v>121</v>
       </c>
       <c r="AF26">
         <v>0</v>
@@ -3119,15 +3187,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:58">
+    <row r="27" spans="1:60">
       <c r="D27" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F27" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -3142,7 +3210,7 @@
         <v>0</v>
       </c>
       <c r="X27" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AF27">
         <v>0</v>
@@ -3193,15 +3261,15 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="28" spans="1:58">
+    <row r="28" spans="1:60">
       <c r="D28" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -3216,7 +3284,7 @@
         <v>0</v>
       </c>
       <c r="X28" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AF28">
         <v>0</v>
@@ -3267,15 +3335,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:58">
+    <row r="29" spans="1:60">
       <c r="D29" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -3338,15 +3406,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:58">
+    <row r="30" spans="1:60">
       <c r="D30" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E30" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -3361,7 +3429,7 @@
         <v>0</v>
       </c>
       <c r="X30" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AF30">
         <v>0</v>
@@ -3412,15 +3480,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:58">
+    <row r="31" spans="1:60">
       <c r="D31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E31" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F31" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -3435,7 +3503,7 @@
         <v>0</v>
       </c>
       <c r="X31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AF31">
         <v>0</v>
@@ -3486,15 +3554,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:58">
+    <row r="32" spans="1:60">
       <c r="D32" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F32" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -3509,7 +3577,7 @@
         <v>0</v>
       </c>
       <c r="X32" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AF32">
         <v>0</v>
@@ -3560,15 +3628,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:58">
+    <row r="33" spans="1:60">
       <c r="D33" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F33" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -3631,15 +3699,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:58">
+    <row r="34" spans="1:60">
       <c r="D34" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E34" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F34" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="L34">
         <v>0</v>
@@ -3702,15 +3770,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:58">
+    <row r="35" spans="1:60">
       <c r="D35" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E35" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F35" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -3773,15 +3841,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:58">
+    <row r="36" spans="1:60">
       <c r="D36" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E36" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F36" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="L36">
         <v>0</v>
@@ -3796,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="X36" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AF36">
         <v>0</v>
@@ -3847,15 +3915,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:58">
+    <row r="37" spans="1:60">
       <c r="D37" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E37" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F37" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="L37">
         <v>0</v>
@@ -3918,385 +3986,385 @@
         <v>0</v>
       </c>
       <c r="BD37" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:58">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:60">
       <c r="D38" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E38" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F38" t="s">
+        <v>154</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>0</v>
+      </c>
+      <c r="AF38">
+        <v>0</v>
+      </c>
+      <c r="AG38">
+        <v>0</v>
+      </c>
+      <c r="AH38">
+        <v>0</v>
+      </c>
+      <c r="AI38">
+        <v>0</v>
+      </c>
+      <c r="AJ38">
+        <v>0</v>
+      </c>
+      <c r="AO38">
+        <v>0</v>
+      </c>
+      <c r="AR38">
+        <v>0</v>
+      </c>
+      <c r="AT38">
+        <v>0</v>
+      </c>
+      <c r="AU38">
+        <v>0</v>
+      </c>
+      <c r="AW38">
+        <v>0</v>
+      </c>
+      <c r="AX38">
+        <v>0</v>
+      </c>
+      <c r="AY38">
+        <v>0</v>
+      </c>
+      <c r="AZ38">
+        <v>0</v>
+      </c>
+      <c r="BA38">
+        <v>0</v>
+      </c>
+      <c r="BB38">
+        <v>0</v>
+      </c>
+      <c r="BC38">
+        <v>0</v>
+      </c>
+      <c r="BD38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:60">
+      <c r="D39" t="s">
+        <v>156</v>
+      </c>
+      <c r="E39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" t="s">
+        <v>157</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>0</v>
+      </c>
+      <c r="AF39">
+        <v>0</v>
+      </c>
+      <c r="AG39">
+        <v>0</v>
+      </c>
+      <c r="AH39">
+        <v>0</v>
+      </c>
+      <c r="AI39">
+        <v>0</v>
+      </c>
+      <c r="AJ39">
+        <v>0</v>
+      </c>
+      <c r="AO39">
+        <v>0</v>
+      </c>
+      <c r="AR39">
+        <v>0</v>
+      </c>
+      <c r="AT39">
+        <v>0</v>
+      </c>
+      <c r="AU39">
+        <v>0</v>
+      </c>
+      <c r="AW39">
+        <v>0</v>
+      </c>
+      <c r="AX39">
+        <v>0</v>
+      </c>
+      <c r="AY39">
+        <v>0</v>
+      </c>
+      <c r="AZ39">
+        <v>0</v>
+      </c>
+      <c r="BA39">
+        <v>0</v>
+      </c>
+      <c r="BB39">
+        <v>0</v>
+      </c>
+      <c r="BC39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:60">
+      <c r="D40" t="s">
+        <v>158</v>
+      </c>
+      <c r="E40" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40" t="s">
+        <v>159</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>0</v>
+      </c>
+      <c r="AF40">
+        <v>0</v>
+      </c>
+      <c r="AG40">
+        <v>0</v>
+      </c>
+      <c r="AH40">
+        <v>0</v>
+      </c>
+      <c r="AI40">
+        <v>0</v>
+      </c>
+      <c r="AJ40">
+        <v>0</v>
+      </c>
+      <c r="AO40">
+        <v>0</v>
+      </c>
+      <c r="AR40">
+        <v>0</v>
+      </c>
+      <c r="AT40">
+        <v>0</v>
+      </c>
+      <c r="AU40">
+        <v>0</v>
+      </c>
+      <c r="AW40">
+        <v>0</v>
+      </c>
+      <c r="AX40">
+        <v>0</v>
+      </c>
+      <c r="AY40">
+        <v>0</v>
+      </c>
+      <c r="AZ40">
+        <v>0</v>
+      </c>
+      <c r="BA40">
+        <v>0</v>
+      </c>
+      <c r="BB40">
+        <v>0</v>
+      </c>
+      <c r="BC40">
+        <v>0</v>
+      </c>
+      <c r="BD40" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:60">
+      <c r="D41" t="s">
+        <v>161</v>
+      </c>
+      <c r="E41" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" t="s">
+        <v>162</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <v>0</v>
+      </c>
+      <c r="X41" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF41">
+        <v>0</v>
+      </c>
+      <c r="AG41">
+        <v>0</v>
+      </c>
+      <c r="AH41">
+        <v>0</v>
+      </c>
+      <c r="AI41">
+        <v>0</v>
+      </c>
+      <c r="AJ41">
+        <v>0</v>
+      </c>
+      <c r="AO41">
+        <v>0</v>
+      </c>
+      <c r="AR41">
+        <v>0</v>
+      </c>
+      <c r="AT41">
+        <v>0</v>
+      </c>
+      <c r="AU41">
+        <v>0</v>
+      </c>
+      <c r="AW41">
+        <v>0</v>
+      </c>
+      <c r="AX41">
+        <v>0</v>
+      </c>
+      <c r="AY41">
+        <v>0</v>
+      </c>
+      <c r="AZ41">
+        <v>0</v>
+      </c>
+      <c r="BA41">
+        <v>0</v>
+      </c>
+      <c r="BB41">
+        <v>0</v>
+      </c>
+      <c r="BC41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:60">
+      <c r="D42" t="s">
+        <v>164</v>
+      </c>
+      <c r="E42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" t="s">
+        <v>165</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42">
+        <v>0</v>
+      </c>
+      <c r="AF42">
+        <v>0</v>
+      </c>
+      <c r="AG42">
+        <v>0</v>
+      </c>
+      <c r="AH42">
+        <v>0</v>
+      </c>
+      <c r="AI42">
+        <v>0</v>
+      </c>
+      <c r="AJ42">
+        <v>0</v>
+      </c>
+      <c r="AO42">
+        <v>0</v>
+      </c>
+      <c r="AR42">
+        <v>0</v>
+      </c>
+      <c r="AT42">
+        <v>0</v>
+      </c>
+      <c r="AU42">
+        <v>0</v>
+      </c>
+      <c r="AW42">
+        <v>0</v>
+      </c>
+      <c r="AX42">
+        <v>0</v>
+      </c>
+      <c r="AY42">
+        <v>0</v>
+      </c>
+      <c r="AZ42">
+        <v>0</v>
+      </c>
+      <c r="BA42">
+        <v>0</v>
+      </c>
+      <c r="BB42">
+        <v>0</v>
+      </c>
+      <c r="BC42">
+        <v>0</v>
+      </c>
+      <c r="BD42" t="s">
         <v>152</v>
       </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
-      <c r="V38">
-        <v>0</v>
-      </c>
-      <c r="W38">
-        <v>0</v>
-      </c>
-      <c r="AF38">
-        <v>0</v>
-      </c>
-      <c r="AG38">
-        <v>0</v>
-      </c>
-      <c r="AH38">
-        <v>0</v>
-      </c>
-      <c r="AI38">
-        <v>0</v>
-      </c>
-      <c r="AJ38">
-        <v>0</v>
-      </c>
-      <c r="AO38">
-        <v>0</v>
-      </c>
-      <c r="AR38">
-        <v>0</v>
-      </c>
-      <c r="AT38">
-        <v>0</v>
-      </c>
-      <c r="AU38">
-        <v>0</v>
-      </c>
-      <c r="AW38">
-        <v>0</v>
-      </c>
-      <c r="AX38">
-        <v>0</v>
-      </c>
-      <c r="AY38">
-        <v>0</v>
-      </c>
-      <c r="AZ38">
-        <v>0</v>
-      </c>
-      <c r="BA38">
-        <v>0</v>
-      </c>
-      <c r="BB38">
-        <v>0</v>
-      </c>
-      <c r="BC38">
-        <v>0</v>
-      </c>
-      <c r="BD38" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="39" spans="1:58">
-      <c r="D39" t="s">
-        <v>154</v>
-      </c>
-      <c r="E39" t="s">
-        <v>59</v>
-      </c>
-      <c r="F39" t="s">
-        <v>155</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-      <c r="V39">
-        <v>0</v>
-      </c>
-      <c r="W39">
-        <v>0</v>
-      </c>
-      <c r="AF39">
-        <v>0</v>
-      </c>
-      <c r="AG39">
-        <v>0</v>
-      </c>
-      <c r="AH39">
-        <v>0</v>
-      </c>
-      <c r="AI39">
-        <v>0</v>
-      </c>
-      <c r="AJ39">
-        <v>0</v>
-      </c>
-      <c r="AO39">
-        <v>0</v>
-      </c>
-      <c r="AR39">
-        <v>0</v>
-      </c>
-      <c r="AT39">
-        <v>0</v>
-      </c>
-      <c r="AU39">
-        <v>0</v>
-      </c>
-      <c r="AW39">
-        <v>0</v>
-      </c>
-      <c r="AX39">
-        <v>0</v>
-      </c>
-      <c r="AY39">
-        <v>0</v>
-      </c>
-      <c r="AZ39">
-        <v>0</v>
-      </c>
-      <c r="BA39">
-        <v>0</v>
-      </c>
-      <c r="BB39">
-        <v>0</v>
-      </c>
-      <c r="BC39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:58">
-      <c r="D40" t="s">
-        <v>156</v>
-      </c>
-      <c r="E40" t="s">
-        <v>59</v>
-      </c>
-      <c r="F40" t="s">
-        <v>157</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="V40">
-        <v>0</v>
-      </c>
-      <c r="W40">
-        <v>0</v>
-      </c>
-      <c r="AF40">
-        <v>0</v>
-      </c>
-      <c r="AG40">
-        <v>0</v>
-      </c>
-      <c r="AH40">
-        <v>0</v>
-      </c>
-      <c r="AI40">
-        <v>0</v>
-      </c>
-      <c r="AJ40">
-        <v>0</v>
-      </c>
-      <c r="AO40">
-        <v>0</v>
-      </c>
-      <c r="AR40">
-        <v>0</v>
-      </c>
-      <c r="AT40">
-        <v>0</v>
-      </c>
-      <c r="AU40">
-        <v>0</v>
-      </c>
-      <c r="AW40">
-        <v>0</v>
-      </c>
-      <c r="AX40">
-        <v>0</v>
-      </c>
-      <c r="AY40">
-        <v>0</v>
-      </c>
-      <c r="AZ40">
-        <v>0</v>
-      </c>
-      <c r="BA40">
-        <v>0</v>
-      </c>
-      <c r="BB40">
-        <v>0</v>
-      </c>
-      <c r="BC40">
-        <v>0</v>
-      </c>
-      <c r="BD40" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:58">
-      <c r="D41" t="s">
-        <v>159</v>
-      </c>
-      <c r="E41" t="s">
-        <v>59</v>
-      </c>
-      <c r="F41" t="s">
-        <v>160</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-      <c r="V41">
-        <v>0</v>
-      </c>
-      <c r="W41">
-        <v>0</v>
-      </c>
-      <c r="X41" t="s">
-        <v>161</v>
-      </c>
-      <c r="AF41">
-        <v>0</v>
-      </c>
-      <c r="AG41">
-        <v>0</v>
-      </c>
-      <c r="AH41">
-        <v>0</v>
-      </c>
-      <c r="AI41">
-        <v>0</v>
-      </c>
-      <c r="AJ41">
-        <v>0</v>
-      </c>
-      <c r="AO41">
-        <v>0</v>
-      </c>
-      <c r="AR41">
-        <v>0</v>
-      </c>
-      <c r="AT41">
-        <v>0</v>
-      </c>
-      <c r="AU41">
-        <v>0</v>
-      </c>
-      <c r="AW41">
-        <v>0</v>
-      </c>
-      <c r="AX41">
-        <v>0</v>
-      </c>
-      <c r="AY41">
-        <v>0</v>
-      </c>
-      <c r="AZ41">
-        <v>0</v>
-      </c>
-      <c r="BA41">
-        <v>0</v>
-      </c>
-      <c r="BB41">
-        <v>0</v>
-      </c>
-      <c r="BC41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:58">
-      <c r="D42" t="s">
-        <v>162</v>
-      </c>
-      <c r="E42" t="s">
-        <v>59</v>
-      </c>
-      <c r="F42" t="s">
-        <v>163</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>0</v>
-      </c>
-      <c r="V42">
-        <v>0</v>
-      </c>
-      <c r="W42">
-        <v>0</v>
-      </c>
-      <c r="AF42">
-        <v>0</v>
-      </c>
-      <c r="AG42">
-        <v>0</v>
-      </c>
-      <c r="AH42">
-        <v>0</v>
-      </c>
-      <c r="AI42">
-        <v>0</v>
-      </c>
-      <c r="AJ42">
-        <v>0</v>
-      </c>
-      <c r="AO42">
-        <v>0</v>
-      </c>
-      <c r="AR42">
-        <v>0</v>
-      </c>
-      <c r="AT42">
-        <v>0</v>
-      </c>
-      <c r="AU42">
-        <v>0</v>
-      </c>
-      <c r="AW42">
-        <v>0</v>
-      </c>
-      <c r="AX42">
-        <v>0</v>
-      </c>
-      <c r="AY42">
-        <v>0</v>
-      </c>
-      <c r="AZ42">
-        <v>0</v>
-      </c>
-      <c r="BA42">
-        <v>0</v>
-      </c>
-      <c r="BB42">
-        <v>0</v>
-      </c>
-      <c r="BC42">
-        <v>0</v>
-      </c>
-      <c r="BD42" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="1:58">
+    </row>
+    <row r="43" spans="1:60">
       <c r="D43" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E43" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F43" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="L43">
         <v>0</v>
@@ -4311,7 +4379,7 @@
         <v>0</v>
       </c>
       <c r="AD43" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="AE43">
         <v>0.25</v>
@@ -4368,18 +4436,18 @@
         <v>0</v>
       </c>
       <c r="BD43" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="44" spans="1:58">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:60">
       <c r="D44" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E44" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F44" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="L44">
         <v>0</v>
@@ -4394,7 +4462,7 @@
         <v>0</v>
       </c>
       <c r="AD44" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="AE44">
         <v>0.75</v>
@@ -4451,18 +4519,18 @@
         <v>0</v>
       </c>
       <c r="BD44" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="45" spans="1:58">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:60">
       <c r="D45" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E45" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F45" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="L45">
         <v>0</v>
@@ -4525,15 +4593,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:58">
+    <row r="46" spans="1:60">
       <c r="D46" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F46" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="L46">
         <v>0</v>
@@ -4548,7 +4616,7 @@
         <v>0</v>
       </c>
       <c r="AD46" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AE46">
         <v>0.75</v>
@@ -4605,15 +4673,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="47" spans="1:58">
+    <row r="47" spans="1:60">
       <c r="D47" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E47" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F47" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="L47">
         <v>0</v>
@@ -4628,7 +4696,7 @@
         <v>0</v>
       </c>
       <c r="X47" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AF47">
         <v>0</v>
@@ -4679,15 +4747,15 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="48" spans="1:58">
+    <row r="48" spans="1:60">
       <c r="D48" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E48" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F48" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="L48">
         <v>0</v>
@@ -4702,7 +4770,7 @@
         <v>0</v>
       </c>
       <c r="X48" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="AF48">
         <v>0</v>
@@ -4753,15 +4821,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:58">
+    <row r="49" spans="1:60">
       <c r="D49" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E49" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F49" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -4824,15 +4892,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:58">
+    <row r="50" spans="1:60">
       <c r="D50" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E50" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F50" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="L50">
         <v>0</v>
@@ -4895,18 +4963,18 @@
         <v>0</v>
       </c>
       <c r="BD50" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="51" spans="1:58">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:60">
       <c r="D51" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E51" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F51" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="L51">
         <v>0</v>
@@ -4969,15 +5037,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:58">
+    <row r="52" spans="1:60">
       <c r="D52" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F52" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="L52">
         <v>0</v>
@@ -5040,18 +5108,18 @@
         <v>0</v>
       </c>
       <c r="BD52" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="53" spans="1:58">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="1:60">
       <c r="D53" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E53" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F53" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="L53">
         <v>0</v>
@@ -5114,15 +5182,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:58">
+    <row r="54" spans="1:60">
       <c r="D54" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E54" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F54" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="L54">
         <v>0</v>
@@ -5185,15 +5253,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:58">
+    <row r="55" spans="1:60">
       <c r="D55" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E55" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F55" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="L55">
         <v>0</v>
@@ -5256,18 +5324,18 @@
         <v>0</v>
       </c>
       <c r="BD55" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="56" spans="1:58">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:60">
       <c r="D56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E56" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="L56">
         <v>0</v>
@@ -5330,18 +5398,18 @@
         <v>0</v>
       </c>
       <c r="BD56" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="57" spans="1:58">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:60">
       <c r="D57" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E57" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F57" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="L57">
         <v>0</v>
@@ -5404,18 +5472,18 @@
         <v>0</v>
       </c>
       <c r="BD57" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="58" spans="1:58">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="1:60">
       <c r="D58" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E58" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F58" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="L58">
         <v>0</v>
@@ -5481,15 +5549,15 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="59" spans="1:58">
+    <row r="59" spans="1:60">
       <c r="D59" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E59" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F59" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="L59">
         <v>0</v>
@@ -5552,18 +5620,18 @@
         <v>0</v>
       </c>
       <c r="BD59" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="60" spans="1:58">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" spans="1:60">
       <c r="D60" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E60" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F60" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="L60">
         <v>0</v>
@@ -5626,18 +5694,18 @@
         <v>0</v>
       </c>
       <c r="BD60" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="61" spans="1:58">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="61" spans="1:60">
       <c r="D61" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E61" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F61" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="L61">
         <v>0</v>
@@ -5700,18 +5768,18 @@
         <v>0</v>
       </c>
       <c r="BD61" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="62" spans="1:58">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:60">
       <c r="D62" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E62" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F62" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="L62">
         <v>0</v>
@@ -5777,15 +5845,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="63" spans="1:58">
+    <row r="63" spans="1:60">
       <c r="D63" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E63" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F63" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="L63">
         <v>0</v>
@@ -5848,18 +5916,18 @@
         <v>0</v>
       </c>
       <c r="BD63" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="64" spans="1:58">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:60">
       <c r="D64" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E64" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F64" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="L64">
         <v>0</v>
@@ -5925,15 +5993,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:58">
+    <row r="65" spans="1:60">
       <c r="D65" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E65" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F65" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="L65">
         <v>0</v>
@@ -5945,21 +6013,69 @@
         <v>0</v>
       </c>
       <c r="W65">
+        <v>0</v>
+      </c>
+      <c r="AF65">
+        <v>0</v>
+      </c>
+      <c r="AG65">
+        <v>0</v>
+      </c>
+      <c r="AH65">
+        <v>0</v>
+      </c>
+      <c r="AI65">
+        <v>0</v>
+      </c>
+      <c r="AJ65">
+        <v>0</v>
+      </c>
+      <c r="AO65">
+        <v>0</v>
+      </c>
+      <c r="AR65">
+        <v>0</v>
+      </c>
+      <c r="AT65">
+        <v>0</v>
+      </c>
+      <c r="AU65">
+        <v>0</v>
+      </c>
+      <c r="AW65">
+        <v>0</v>
+      </c>
+      <c r="AX65">
+        <v>0</v>
+      </c>
+      <c r="AY65">
+        <v>0</v>
+      </c>
+      <c r="AZ65">
+        <v>0</v>
+      </c>
+      <c r="BA65">
+        <v>0</v>
+      </c>
+      <c r="BB65">
+        <v>0</v>
+      </c>
+      <c r="BC65">
         <v>0</v>
       </c>
       <c r="BE65">
         <v>0.05</v>
       </c>
     </row>
-    <row r="66" spans="1:58">
+    <row r="66" spans="1:60">
       <c r="D66" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E66" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F66" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="L66">
         <v>0</v>
@@ -5971,21 +6087,69 @@
         <v>0</v>
       </c>
       <c r="W66">
+        <v>0</v>
+      </c>
+      <c r="AF66">
+        <v>0</v>
+      </c>
+      <c r="AG66">
+        <v>0</v>
+      </c>
+      <c r="AH66">
+        <v>0</v>
+      </c>
+      <c r="AI66">
+        <v>0</v>
+      </c>
+      <c r="AJ66">
+        <v>0</v>
+      </c>
+      <c r="AO66">
+        <v>0</v>
+      </c>
+      <c r="AR66">
+        <v>0</v>
+      </c>
+      <c r="AT66">
+        <v>0</v>
+      </c>
+      <c r="AU66">
+        <v>0</v>
+      </c>
+      <c r="AW66">
+        <v>0</v>
+      </c>
+      <c r="AX66">
+        <v>0</v>
+      </c>
+      <c r="AY66">
+        <v>0</v>
+      </c>
+      <c r="AZ66">
+        <v>0</v>
+      </c>
+      <c r="BA66">
+        <v>0</v>
+      </c>
+      <c r="BB66">
+        <v>0</v>
+      </c>
+      <c r="BC66">
         <v>0</v>
       </c>
       <c r="BE66">
         <v>0.8</v>
       </c>
     </row>
-    <row r="67" spans="1:58">
+    <row r="67" spans="1:60">
       <c r="D67" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E67" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F67" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="L67">
         <v>0</v>
@@ -6000,18 +6164,66 @@
         <v>0</v>
       </c>
       <c r="X67" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="68" spans="1:58">
+        <v>223</v>
+      </c>
+      <c r="AF67">
+        <v>0</v>
+      </c>
+      <c r="AG67">
+        <v>0</v>
+      </c>
+      <c r="AH67">
+        <v>0</v>
+      </c>
+      <c r="AI67">
+        <v>0</v>
+      </c>
+      <c r="AJ67">
+        <v>0</v>
+      </c>
+      <c r="AO67">
+        <v>0</v>
+      </c>
+      <c r="AR67">
+        <v>0</v>
+      </c>
+      <c r="AT67">
+        <v>0</v>
+      </c>
+      <c r="AU67">
+        <v>0</v>
+      </c>
+      <c r="AW67">
+        <v>0</v>
+      </c>
+      <c r="AX67">
+        <v>0</v>
+      </c>
+      <c r="AY67">
+        <v>0</v>
+      </c>
+      <c r="AZ67">
+        <v>0</v>
+      </c>
+      <c r="BA67">
+        <v>0</v>
+      </c>
+      <c r="BB67">
+        <v>0</v>
+      </c>
+      <c r="BC67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:60">
       <c r="D68" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E68" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F68" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="L68">
         <v>0</v>
@@ -6025,19 +6237,67 @@
       <c r="W68">
         <v>0</v>
       </c>
+      <c r="AF68">
+        <v>0</v>
+      </c>
+      <c r="AG68">
+        <v>0</v>
+      </c>
+      <c r="AH68">
+        <v>0</v>
+      </c>
+      <c r="AI68">
+        <v>0</v>
+      </c>
+      <c r="AJ68">
+        <v>0</v>
+      </c>
+      <c r="AO68">
+        <v>0</v>
+      </c>
+      <c r="AR68">
+        <v>0</v>
+      </c>
+      <c r="AT68">
+        <v>0</v>
+      </c>
+      <c r="AU68">
+        <v>0</v>
+      </c>
+      <c r="AW68">
+        <v>0</v>
+      </c>
+      <c r="AX68">
+        <v>0</v>
+      </c>
+      <c r="AY68">
+        <v>0</v>
+      </c>
+      <c r="AZ68">
+        <v>0</v>
+      </c>
+      <c r="BA68">
+        <v>0</v>
+      </c>
+      <c r="BB68">
+        <v>0</v>
+      </c>
+      <c r="BC68">
+        <v>0</v>
+      </c>
       <c r="BD68" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="69" spans="1:58">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:60">
       <c r="D69" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E69" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F69" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="L69">
         <v>0</v>
@@ -6051,19 +6311,67 @@
       <c r="W69">
         <v>0</v>
       </c>
+      <c r="AF69">
+        <v>0</v>
+      </c>
+      <c r="AG69">
+        <v>0</v>
+      </c>
+      <c r="AH69">
+        <v>0</v>
+      </c>
+      <c r="AI69">
+        <v>0</v>
+      </c>
+      <c r="AJ69">
+        <v>0</v>
+      </c>
+      <c r="AO69">
+        <v>0</v>
+      </c>
+      <c r="AR69">
+        <v>0</v>
+      </c>
+      <c r="AT69">
+        <v>0</v>
+      </c>
+      <c r="AU69">
+        <v>0</v>
+      </c>
+      <c r="AW69">
+        <v>0</v>
+      </c>
+      <c r="AX69">
+        <v>0</v>
+      </c>
+      <c r="AY69">
+        <v>0</v>
+      </c>
+      <c r="AZ69">
+        <v>0</v>
+      </c>
+      <c r="BA69">
+        <v>0</v>
+      </c>
+      <c r="BB69">
+        <v>0</v>
+      </c>
+      <c r="BC69">
+        <v>0</v>
+      </c>
       <c r="BD69" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="70" spans="1:58">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="70" spans="1:60">
       <c r="D70" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E70" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F70" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L70">
         <v>0</v>
@@ -6077,16 +6385,64 @@
       <c r="W70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:58">
+      <c r="AF70">
+        <v>0</v>
+      </c>
+      <c r="AG70">
+        <v>0</v>
+      </c>
+      <c r="AH70">
+        <v>0</v>
+      </c>
+      <c r="AI70">
+        <v>0</v>
+      </c>
+      <c r="AJ70">
+        <v>0</v>
+      </c>
+      <c r="AO70">
+        <v>0</v>
+      </c>
+      <c r="AR70">
+        <v>0</v>
+      </c>
+      <c r="AT70">
+        <v>0</v>
+      </c>
+      <c r="AU70">
+        <v>0</v>
+      </c>
+      <c r="AW70">
+        <v>0</v>
+      </c>
+      <c r="AX70">
+        <v>0</v>
+      </c>
+      <c r="AY70">
+        <v>0</v>
+      </c>
+      <c r="AZ70">
+        <v>0</v>
+      </c>
+      <c r="BA70">
+        <v>0</v>
+      </c>
+      <c r="BB70">
+        <v>0</v>
+      </c>
+      <c r="BC70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:60">
       <c r="D71" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E71" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F71" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="L71">
         <v>0</v>
@@ -6101,18 +6457,66 @@
         <v>0</v>
       </c>
       <c r="X71" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="72" spans="1:58">
+        <v>232</v>
+      </c>
+      <c r="AF71">
+        <v>0</v>
+      </c>
+      <c r="AG71">
+        <v>0</v>
+      </c>
+      <c r="AH71">
+        <v>0</v>
+      </c>
+      <c r="AI71">
+        <v>0</v>
+      </c>
+      <c r="AJ71">
+        <v>0</v>
+      </c>
+      <c r="AO71">
+        <v>0</v>
+      </c>
+      <c r="AR71">
+        <v>0</v>
+      </c>
+      <c r="AT71">
+        <v>0</v>
+      </c>
+      <c r="AU71">
+        <v>0</v>
+      </c>
+      <c r="AW71">
+        <v>0</v>
+      </c>
+      <c r="AX71">
+        <v>0</v>
+      </c>
+      <c r="AY71">
+        <v>0</v>
+      </c>
+      <c r="AZ71">
+        <v>0</v>
+      </c>
+      <c r="BA71">
+        <v>0</v>
+      </c>
+      <c r="BB71">
+        <v>0</v>
+      </c>
+      <c r="BC71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:60">
       <c r="D72" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E72" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F72" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="L72">
         <v>0</v>
@@ -6126,8 +6530,56 @@
       <c r="W72">
         <v>0</v>
       </c>
+      <c r="AF72">
+        <v>0</v>
+      </c>
+      <c r="AG72">
+        <v>0</v>
+      </c>
+      <c r="AH72">
+        <v>0</v>
+      </c>
+      <c r="AI72">
+        <v>0</v>
+      </c>
+      <c r="AJ72">
+        <v>0</v>
+      </c>
+      <c r="AO72">
+        <v>0</v>
+      </c>
+      <c r="AR72">
+        <v>0</v>
+      </c>
+      <c r="AT72">
+        <v>0</v>
+      </c>
+      <c r="AU72">
+        <v>0</v>
+      </c>
+      <c r="AW72">
+        <v>0</v>
+      </c>
+      <c r="AX72">
+        <v>0</v>
+      </c>
+      <c r="AY72">
+        <v>0</v>
+      </c>
+      <c r="AZ72">
+        <v>0</v>
+      </c>
+      <c r="BA72">
+        <v>0</v>
+      </c>
+      <c r="BB72">
+        <v>0</v>
+      </c>
+      <c r="BC72">
+        <v>0</v>
+      </c>
       <c r="BD72" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="BE72">
         <v>0.05</v>
@@ -6136,15 +6588,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:58">
+    <row r="73" spans="1:60">
       <c r="D73" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E73" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F73" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="L73">
         <v>0</v>
@@ -6156,6 +6608,54 @@
         <v>0</v>
       </c>
       <c r="W73">
+        <v>0</v>
+      </c>
+      <c r="AF73">
+        <v>0</v>
+      </c>
+      <c r="AG73">
+        <v>0</v>
+      </c>
+      <c r="AH73">
+        <v>0</v>
+      </c>
+      <c r="AI73">
+        <v>0</v>
+      </c>
+      <c r="AJ73">
+        <v>0</v>
+      </c>
+      <c r="AO73">
+        <v>0</v>
+      </c>
+      <c r="AR73">
+        <v>0</v>
+      </c>
+      <c r="AT73">
+        <v>0</v>
+      </c>
+      <c r="AU73">
+        <v>0</v>
+      </c>
+      <c r="AW73">
+        <v>0</v>
+      </c>
+      <c r="AX73">
+        <v>0</v>
+      </c>
+      <c r="AY73">
+        <v>0</v>
+      </c>
+      <c r="AZ73">
+        <v>0</v>
+      </c>
+      <c r="BA73">
+        <v>0</v>
+      </c>
+      <c r="BB73">
+        <v>0</v>
+      </c>
+      <c r="BC73">
         <v>0</v>
       </c>
       <c r="BE73">
@@ -6165,15 +6665,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:58">
+    <row r="74" spans="1:60">
       <c r="D74" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E74" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F74" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="L74">
         <v>0</v>
@@ -6187,8 +6687,56 @@
       <c r="W74">
         <v>0</v>
       </c>
+      <c r="AF74">
+        <v>0</v>
+      </c>
+      <c r="AG74">
+        <v>0</v>
+      </c>
+      <c r="AH74">
+        <v>0</v>
+      </c>
+      <c r="AI74">
+        <v>0</v>
+      </c>
+      <c r="AJ74">
+        <v>0</v>
+      </c>
+      <c r="AO74">
+        <v>0</v>
+      </c>
+      <c r="AR74">
+        <v>0</v>
+      </c>
+      <c r="AT74">
+        <v>0</v>
+      </c>
+      <c r="AU74">
+        <v>0</v>
+      </c>
+      <c r="AW74">
+        <v>0</v>
+      </c>
+      <c r="AX74">
+        <v>0</v>
+      </c>
+      <c r="AY74">
+        <v>0</v>
+      </c>
+      <c r="AZ74">
+        <v>0</v>
+      </c>
+      <c r="BA74">
+        <v>0</v>
+      </c>
+      <c r="BB74">
+        <v>0</v>
+      </c>
+      <c r="BC74">
+        <v>0</v>
+      </c>
       <c r="BD74" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="BE74">
         <v>0.15</v>
@@ -6197,15 +6745,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:58">
+    <row r="75" spans="1:60">
       <c r="D75" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E75" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F75" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="L75">
         <v>0</v>
@@ -6217,6 +6765,54 @@
         <v>0</v>
       </c>
       <c r="W75">
+        <v>0</v>
+      </c>
+      <c r="AF75">
+        <v>0</v>
+      </c>
+      <c r="AG75">
+        <v>0</v>
+      </c>
+      <c r="AH75">
+        <v>0</v>
+      </c>
+      <c r="AI75">
+        <v>0</v>
+      </c>
+      <c r="AJ75">
+        <v>0</v>
+      </c>
+      <c r="AO75">
+        <v>0</v>
+      </c>
+      <c r="AR75">
+        <v>0</v>
+      </c>
+      <c r="AT75">
+        <v>0</v>
+      </c>
+      <c r="AU75">
+        <v>0</v>
+      </c>
+      <c r="AW75">
+        <v>0</v>
+      </c>
+      <c r="AX75">
+        <v>0</v>
+      </c>
+      <c r="AY75">
+        <v>0</v>
+      </c>
+      <c r="AZ75">
+        <v>0</v>
+      </c>
+      <c r="BA75">
+        <v>0</v>
+      </c>
+      <c r="BB75">
+        <v>0</v>
+      </c>
+      <c r="BC75">
         <v>0</v>
       </c>
       <c r="BE75">
@@ -6226,15 +6822,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:58">
+    <row r="76" spans="1:60">
       <c r="D76" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E76" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F76" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="L76">
         <v>0</v>
@@ -6246,6 +6842,54 @@
         <v>0</v>
       </c>
       <c r="W76">
+        <v>0</v>
+      </c>
+      <c r="AF76">
+        <v>0</v>
+      </c>
+      <c r="AG76">
+        <v>0</v>
+      </c>
+      <c r="AH76">
+        <v>0</v>
+      </c>
+      <c r="AI76">
+        <v>0</v>
+      </c>
+      <c r="AJ76">
+        <v>0</v>
+      </c>
+      <c r="AO76">
+        <v>0</v>
+      </c>
+      <c r="AR76">
+        <v>0</v>
+      </c>
+      <c r="AT76">
+        <v>0</v>
+      </c>
+      <c r="AU76">
+        <v>0</v>
+      </c>
+      <c r="AW76">
+        <v>0</v>
+      </c>
+      <c r="AX76">
+        <v>0</v>
+      </c>
+      <c r="AY76">
+        <v>0</v>
+      </c>
+      <c r="AZ76">
+        <v>0</v>
+      </c>
+      <c r="BA76">
+        <v>0</v>
+      </c>
+      <c r="BB76">
+        <v>0</v>
+      </c>
+      <c r="BC76">
         <v>0</v>
       </c>
       <c r="BE76">
@@ -6253,6 +6897,243 @@
       </c>
       <c r="BF76">
         <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:60">
+      <c r="D77" t="s">
+        <v>243</v>
+      </c>
+      <c r="E77" t="s">
+        <v>61</v>
+      </c>
+      <c r="F77" t="s">
+        <v>244</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="V77">
+        <v>0</v>
+      </c>
+      <c r="W77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:60">
+      <c r="D78" t="s">
+        <v>245</v>
+      </c>
+      <c r="E78" t="s">
+        <v>61</v>
+      </c>
+      <c r="F78" t="s">
+        <v>246</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="V78">
+        <v>0</v>
+      </c>
+      <c r="W78">
+        <v>0</v>
+      </c>
+      <c r="BD78" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:60">
+      <c r="D79" t="s">
+        <v>247</v>
+      </c>
+      <c r="E79" t="s">
+        <v>61</v>
+      </c>
+      <c r="F79" t="s">
+        <v>248</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="V79">
+        <v>0</v>
+      </c>
+      <c r="W79">
+        <v>0</v>
+      </c>
+      <c r="BD79" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="80" spans="1:60">
+      <c r="D80" t="s">
+        <v>249</v>
+      </c>
+      <c r="E80" t="s">
+        <v>61</v>
+      </c>
+      <c r="F80" t="s">
+        <v>250</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="V80">
+        <v>0</v>
+      </c>
+      <c r="W80">
+        <v>0</v>
+      </c>
+      <c r="BD80" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:60">
+      <c r="D81" t="s">
+        <v>251</v>
+      </c>
+      <c r="E81" t="s">
+        <v>61</v>
+      </c>
+      <c r="F81" t="s">
+        <v>252</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81">
+        <v>0</v>
+      </c>
+      <c r="V81">
+        <v>0</v>
+      </c>
+      <c r="W81">
+        <v>0</v>
+      </c>
+      <c r="BD81" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="82" spans="1:60">
+      <c r="D82" t="s">
+        <v>253</v>
+      </c>
+      <c r="E82" t="s">
+        <v>61</v>
+      </c>
+      <c r="F82" t="s">
+        <v>254</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+      <c r="V82">
+        <v>0</v>
+      </c>
+      <c r="W82">
+        <v>0</v>
+      </c>
+      <c r="BE82">
+        <v>0.25</v>
+      </c>
+      <c r="BF82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:60">
+      <c r="D83" t="s">
+        <v>255</v>
+      </c>
+      <c r="E83" t="s">
+        <v>61</v>
+      </c>
+      <c r="F83" t="s">
+        <v>256</v>
+      </c>
+      <c r="L83">
+        <v>0</v>
+      </c>
+      <c r="M83">
+        <v>0</v>
+      </c>
+      <c r="V83">
+        <v>0</v>
+      </c>
+      <c r="W83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:60">
+      <c r="D84" t="s">
+        <v>257</v>
+      </c>
+      <c r="E84" t="s">
+        <v>61</v>
+      </c>
+      <c r="F84" t="s">
+        <v>258</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84">
+        <v>0</v>
+      </c>
+      <c r="V84">
+        <v>0</v>
+      </c>
+      <c r="W84">
+        <v>0</v>
+      </c>
+      <c r="BC84">
+        <v>0.35</v>
+      </c>
+      <c r="BE84">
+        <v>1.6</v>
+      </c>
+      <c r="BF84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:60">
+      <c r="D85" t="s">
+        <v>259</v>
+      </c>
+      <c r="E85" t="s">
+        <v>61</v>
+      </c>
+      <c r="F85" t="s">
+        <v>260</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85">
+        <v>0</v>
+      </c>
+      <c r="V85">
+        <v>0</v>
+      </c>
+      <c r="W85">
+        <v>0</v>
+      </c>
+      <c r="BD85" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>